<commit_message>
Shift Rota Generation - Bug fixing with Lists
</commit_message>
<xml_diff>
--- a/Rota/c5_rota.xlsx
+++ b/Rota/c5_rota.xlsx
@@ -506,7 +506,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -534,7 +534,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -544,7 +544,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>
@@ -567,12 +567,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Sushvin</t>
         </is>
       </c>
     </row>
@@ -590,12 +590,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -618,17 +618,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>
@@ -646,17 +646,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
     </row>
@@ -674,17 +674,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Sushvin</t>
         </is>
       </c>
     </row>
@@ -702,7 +702,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -712,7 +712,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Kapil</t>
         </is>
       </c>
     </row>
@@ -758,12 +758,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -786,17 +786,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>
@@ -814,17 +814,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Sushvin</t>
         </is>
       </c>
     </row>
@@ -852,7 +852,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Sushvin</t>
         </is>
       </c>
     </row>
@@ -870,17 +870,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Divik</t>
         </is>
       </c>
     </row>
@@ -898,17 +898,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Divik</t>
         </is>
       </c>
     </row>
@@ -931,12 +931,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>
@@ -954,7 +954,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -982,17 +982,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
     </row>
@@ -1010,17 +1010,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Divik</t>
         </is>
       </c>
     </row>
@@ -1043,12 +1043,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Shift Rota Generation - Final delivery
</commit_message>
<xml_diff>
--- a/Rota/c5_rota.xlsx
+++ b/Rota/c5_rota.xlsx
@@ -460,7 +460,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>BAS_FinC</t>
+          <t>BAS_Finance</t>
         </is>
       </c>
     </row>
@@ -506,17 +506,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Sushvin</t>
         </is>
       </c>
     </row>
@@ -534,17 +534,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Kapil</t>
         </is>
       </c>
     </row>
@@ -562,7 +562,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -572,7 +572,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -618,7 +618,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -628,7 +628,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Sushvin</t>
         </is>
       </c>
     </row>
@@ -646,17 +646,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Divik</t>
         </is>
       </c>
     </row>
@@ -674,7 +674,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -684,7 +684,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
     </row>
@@ -707,12 +707,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Sushvin</t>
         </is>
       </c>
     </row>
@@ -730,17 +730,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>
@@ -758,17 +758,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Sushvin</t>
         </is>
       </c>
     </row>
@@ -786,17 +786,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Kapil</t>
         </is>
       </c>
     </row>
@@ -814,17 +814,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>
@@ -842,17 +842,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Divik</t>
         </is>
       </c>
     </row>
@@ -870,17 +870,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>
@@ -903,7 +903,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -931,12 +931,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Sushvin</t>
         </is>
       </c>
     </row>
@@ -954,12 +954,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -982,17 +982,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>
@@ -1015,12 +1015,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Sushvin</t>
         </is>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Kapil</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Shift Rota Generation - Final delivery with equal distribution
</commit_message>
<xml_diff>
--- a/Rota/c5_rota.xlsx
+++ b/Rota/c5_rota.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,7 +511,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -534,17 +534,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>
@@ -567,12 +567,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Kapil</t>
         </is>
       </c>
     </row>
@@ -590,12 +590,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -618,7 +618,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -628,7 +628,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>
@@ -656,7 +656,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Sushvin</t>
         </is>
       </c>
     </row>
@@ -674,17 +674,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>
@@ -702,17 +702,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
     </row>
@@ -730,17 +730,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Sushvin</t>
         </is>
       </c>
     </row>
@@ -758,7 +758,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -768,7 +768,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>
@@ -786,7 +786,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Divik</t>
         </is>
       </c>
     </row>
@@ -814,7 +814,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Kapil</t>
         </is>
       </c>
     </row>
@@ -847,12 +847,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Sushvin</t>
         </is>
       </c>
     </row>
@@ -870,17 +870,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Kapil</t>
         </is>
       </c>
     </row>
@@ -926,17 +926,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Kapil</t>
+          <t>Sushvin</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Divik</t>
+          <t>Naveen</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
     </row>
@@ -954,101 +954,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Naveen</t>
+          <t>Divik</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Sushvin</t>
+          <t>Kapil</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Kapil</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2" t="n">
-        <v>44382</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Divik</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Kapil</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Naveen</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2" t="n">
-        <v>44389</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Kapil</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Naveen</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Sushvin</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>44396</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Sushvin</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Divik</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Kapil</t>
+          <t>Naveen</t>
         </is>
       </c>
     </row>

</xml_diff>